<commit_message>
Major modifications Change config locations, changed app to my counter app.Implemented failure screenshot
</commit_message>
<xml_diff>
--- a/src/test/java/com/testData/LoginData.xlsx
+++ b/src/test/java/com/testData/LoginData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A83809-B41C-4823-BF23-D571DF8FE846}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18035986-0066-40B0-A836-4FA36C90F431}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35385" yWindow="3420" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,36 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>mngr83460</t>
+    <t>clicks</t>
   </si>
   <si>
-    <t>qAbUzyj</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>mngr112909</t>
-  </si>
-  <si>
-    <t>tytUreg</t>
-  </si>
-  <si>
-    <t>mngr137319</t>
-  </si>
-  <si>
-    <t>bAdYvyb</t>
-  </si>
-  <si>
-    <t>mngr164225</t>
-  </si>
-  <si>
-    <t>jahetAp</t>
+    <t>counts</t>
   </si>
 </sst>
 </file>
@@ -442,7 +418,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,50 +429,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="B4" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
+      <c r="A6" s="2">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>